<commit_message>
tested v1. v2, v3 and all are working. Changed the TOOLBOX in V3 to TOOLBOX_ALPHA in the .env file. DIDNT change the path in the call routine
</commit_message>
<xml_diff>
--- a/autoast/Cariboo_replacement_2_jobs.xlsx
+++ b/autoast/Cariboo_replacement_2_jobs.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,12 +29,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
       <sz val="11"/>
     </font>
     <font>
@@ -101,7 +95,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -130,19 +124,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -557,19 +542,19 @@
   <cols>
     <col width="23.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
     <col width="138.8621428571429" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
-    <col width="17.71928571428571" bestFit="1" customWidth="1" style="16" min="3" max="3"/>
-    <col width="16.86214285714286" bestFit="1" customWidth="1" style="16" min="4" max="4"/>
-    <col width="17.29071428571428" bestFit="1" customWidth="1" style="16" min="5" max="5"/>
+    <col width="17.71928571428571" bestFit="1" customWidth="1" style="13" min="3" max="3"/>
+    <col width="16.86214285714286" bestFit="1" customWidth="1" style="13" min="4" max="4"/>
+    <col width="17.29071428571428" bestFit="1" customWidth="1" style="13" min="5" max="5"/>
     <col width="110.4335714285714" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
-    <col width="29.29071428571428" bestFit="1" customWidth="1" style="17" min="7" max="7"/>
-    <col width="20.57642857142857" bestFit="1" customWidth="1" style="17" min="8" max="8"/>
-    <col width="25.57642857142857" bestFit="1" customWidth="1" style="17" min="9" max="9"/>
-    <col width="21.005" bestFit="1" customWidth="1" style="17" min="10" max="10"/>
-    <col width="21.29071428571428" bestFit="1" customWidth="1" style="17" min="11" max="11"/>
-    <col width="13.71928571428571" bestFit="1" customWidth="1" style="17" min="12" max="12"/>
+    <col width="29.29071428571428" bestFit="1" customWidth="1" style="14" min="7" max="7"/>
+    <col width="20.57642857142857" bestFit="1" customWidth="1" style="14" min="8" max="8"/>
+    <col width="25.57642857142857" bestFit="1" customWidth="1" style="14" min="9" max="9"/>
+    <col width="21.005" bestFit="1" customWidth="1" style="14" min="10" max="10"/>
+    <col width="21.29071428571428" bestFit="1" customWidth="1" style="14" min="11" max="11"/>
+    <col width="13.71928571428571" bestFit="1" customWidth="1" style="14" min="12" max="12"/>
     <col width="14.71928571428571" bestFit="1" customWidth="1" style="5" min="13" max="13"/>
     <col width="11.57642857142857" bestFit="1" customWidth="1" style="5" min="14" max="14"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="18" min="15" max="15"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="15" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -651,7 +636,7 @@
           <t>Cariboo</t>
         </is>
       </c>
-      <c r="B2" s="10" t="n"/>
+      <c r="B2" s="3" t="n"/>
       <c r="C2" s="7" t="inlineStr">
         <is>
           <t>0307321</t>
@@ -702,13 +687,13 @@
           <t>true</t>
         </is>
       </c>
-      <c r="M2" s="11" t="inlineStr">
-        <is>
-          <t>COMPLETE</t>
-        </is>
-      </c>
-      <c r="N2" s="10" t="n"/>
-      <c r="O2" s="12" t="n"/>
+      <c r="M2" s="10" t="inlineStr">
+        <is>
+          <t>Queued</t>
+        </is>
+      </c>
+      <c r="N2" s="3" t="n"/>
+      <c r="O2" s="9" t="n"/>
     </row>
     <row r="3" ht="19.5" customHeight="1">
       <c r="A3" s="3" t="inlineStr">
@@ -716,7 +701,7 @@
           <t>Cariboo</t>
         </is>
       </c>
-      <c r="B3" s="13" t="n"/>
+      <c r="B3" s="11" t="n"/>
       <c r="C3" s="7" t="inlineStr">
         <is>
           <t>3401246</t>
@@ -767,12 +752,12 @@
           <t>true</t>
         </is>
       </c>
-      <c r="M3" s="14" t="inlineStr">
-        <is>
-          <t>COMPLETE</t>
-        </is>
-      </c>
-      <c r="N3" s="15" t="n"/>
+      <c r="M3" s="10" t="inlineStr">
+        <is>
+          <t>Queued</t>
+        </is>
+      </c>
+      <c r="N3" s="12" t="n"/>
       <c r="O3" s="9" t="n"/>
     </row>
   </sheetData>

</xml_diff>